<commit_message>
clean up on BUH and Sales team roles
</commit_message>
<xml_diff>
--- a/sample_csv/customer_data.xlsx
+++ b/sample_csv/customer_data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win10\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghuvallikkat/Desktop/LEADSOC_CODE/CRM1.0/sample_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFAE18B-6775-4883-8AA5-64FBE71AEC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559DE7CD-CFDF-0347-A472-AF6AC8B3E80F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAE5679E-1ABB-421C-8A94-258CD2E0AC13}"/>
+    <workbookView xWindow="4300" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{DAE5679E-1ABB-421C-8A94-258CD2E0AC13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>cName</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Cisco</t>
+  </si>
+  <si>
+    <t>LeadSoc</t>
+  </si>
+  <si>
+    <t>leadsoc@gmail.com</t>
+  </si>
+  <si>
+    <t>www.leadsoc.com</t>
   </si>
 </sst>
 </file>
@@ -498,19 +507,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B498A7D1-B950-44F6-88E6-AC62A751F016}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" activeCellId="1" sqref="A2:D13 B1:D1"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -532,7 +541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -543,7 +552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -554,7 +563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -565,7 +574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -576,7 +585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -587,7 +596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -598,7 +607,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -609,7 +618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -620,7 +629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -631,7 +640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -642,7 +651,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -651,6 +660,17 @@
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -679,6 +699,8 @@
     <hyperlink ref="C12" r:id="rId22" xr:uid="{CA65FA4E-E967-4CD2-8902-B112C610DD8D}"/>
     <hyperlink ref="B13" r:id="rId23" xr:uid="{C7AADEAC-4B34-4374-8E0E-CBCABBC07A1A}"/>
     <hyperlink ref="C13" r:id="rId24" xr:uid="{CBE79F0B-557E-4BF6-B78F-569A1D71C72E}"/>
+    <hyperlink ref="B14" r:id="rId25" xr:uid="{B846F9F4-D588-A64D-B00F-8EB438254EA6}"/>
+    <hyperlink ref="C14" r:id="rId26" xr:uid="{C69048A5-91A9-334C-A531-2E05146EF1AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>